<commit_message>
Atualização na documentação e PBL
</commit_message>
<xml_diff>
--- a/Documentação/Backlog_CyberWise.xlsx
+++ b/Documentação/Backlog_CyberWise.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davif\Desktop\faculdade\2 semestre\CyberWise\cyberwise\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2774502-62ED-406C-9554-1E7E4F009D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2500C8-E158-48B0-9F3F-42505032CDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="83">
   <si>
     <t>Descrição</t>
   </si>
@@ -276,13 +276,22 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema para enviar notificação via slack </t>
+  </si>
+  <si>
+    <t>Cliente linux com permissões configuradas</t>
+  </si>
+  <si>
+    <t>User Stories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +370,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -400,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -824,11 +839,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF191D12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1107,12 +1131,49 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1496,7 +1557,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Tecnosolo" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1519,13 +1580,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requisitos" displayName="Requisitos" ref="A1:I38" headerRowDxfId="14" dataDxfId="12" totalsRowDxfId="10" headerRowBorderDxfId="13" tableBorderDxfId="11">
-  <autoFilter ref="A1:I38" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requisitos" displayName="Requisitos" ref="A1:J38" headerRowDxfId="15" dataDxfId="13" totalsRowDxfId="11" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A1:J38" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1535,22 +1592,24 @@
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I35">
-    <sortCondition ref="I2:I35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J35">
+    <sortCondition ref="J2:J35"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="5" xr3:uid="{00FA1D34-6EA6-4C9C-926C-8002D0A7239E}" name="ID" dataDxfId="9" totalsRowDxfId="8">
+  <tableColumns count="10">
+    <tableColumn id="5" xr3:uid="{00FA1D34-6EA6-4C9C-926C-8002D0A7239E}" name="ID" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" totalsRowLabel="Total" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Funcionalidade" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Classificação" totalsRowFunction="count" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tamanho" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tamanho (Number)" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Prioridade" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Sprint" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Requisito" totalsRowLabel="Total" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Funcionalidade" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Classificação" totalsRowFunction="count" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tamanho" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tamanho (Number)" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Prioridade" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{88427A5E-7B16-4FCA-983F-BAEBEE9770BD}" name="User Stories" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Sprint" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Tecnosolo" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1853,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DN1048575"/>
+  <dimension ref="A1:DO1048575"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="52" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,14 +1928,16 @@
     <col min="6" max="6" width="28.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.5546875" customWidth="1"/>
     <col min="8" max="8" width="27.21875" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="16" max="16" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.21875" customWidth="1"/>
-    <col min="18" max="18" width="42.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" customWidth="1"/>
+    <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="94" t="s">
         <v>20</v>
       </c>
@@ -1902,10 +1963,13 @@
         <v>78</v>
       </c>
       <c r="I1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="90">
         <f t="shared" ref="A2:A38" si="0">ROW(A1)</f>
         <v>1</v>
@@ -1931,18 +1995,12 @@
       <c r="H2" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="95"/>
+      <c r="J2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="R2" s="6">
-        <f>SUM(G2:G28)</f>
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:44" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="87">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1968,18 +2026,12 @@
       <c r="H3" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="50" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="53">
-        <f>SUM(G6,G8,G14)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:44" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="87">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2005,18 +2057,12 @@
       <c r="H4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="96"/>
+      <c r="J4" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" s="54" t="e">
-        <f>SUM(G2,G3,G4,G5,G9,G10,G11,G23,G25,#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:44" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2042,18 +2088,12 @@
       <c r="H5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="96"/>
+      <c r="J5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R5" s="54">
-        <f>SUM(G7,G28,G12,G15,G16,G17,G21,G18,G27)</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:44" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2079,19 +2119,13 @@
       <c r="H6" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="49"/>
+      <c r="J6" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="Q6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R6" s="55">
-        <f>SUM(G13,G19,G20,G22,G24,G26)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:44" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="87">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2117,17 +2151,13 @@
       <c r="H7" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="31"/>
+      <c r="J7" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="56" t="e">
-        <f>SUM(R3:R6)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:44" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="87">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2153,14 +2183,13 @@
       <c r="H8" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="37" t="s">
+      <c r="I8" s="95"/>
+      <c r="J8" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="2"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="57"/>
-    </row>
-    <row r="9" spans="1:18" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:44" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2186,12 +2215,13 @@
       <c r="H9" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="95"/>
+      <c r="J9" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:44" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="87">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2217,12 +2247,13 @@
       <c r="H10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="96"/>
+      <c r="J10" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:44" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="88">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2248,12 +2279,13 @@
       <c r="H11" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="64"/>
+      <c r="J11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:44" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="87">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2279,12 +2311,13 @@
       <c r="H12" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="49"/>
+      <c r="J12" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:44" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="87">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2310,11 +2343,12 @@
       <c r="H13" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="31"/>
+      <c r="J13" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="87">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2340,11 +2374,12 @@
       <c r="H14" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="I14" s="31"/>
+      <c r="J14" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="87">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2370,11 +2405,19 @@
       <c r="H15" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I15" s="49"/>
+      <c r="J15" s="33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR15" s="6">
+        <f>SUM(G2:G28)</f>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="88">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2400,11 +2443,19 @@
       <c r="H16" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="I16" s="97"/>
+      <c r="J16" s="37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:118" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR16" s="53">
+        <f>SUM(G6,G8,G14)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:119" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="87">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2430,11 +2481,19 @@
       <c r="H17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="96"/>
+      <c r="J17" s="33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:118" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR17" s="54" t="e">
+        <f>SUM(G2,G3,G4,G5,G9,G10,G11,G23,G25,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:119" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="87">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2460,11 +2519,19 @@
       <c r="H18" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="67" t="s">
+      <c r="I18" s="41"/>
+      <c r="J18" s="67" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:118" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR18" s="54">
+        <f>SUM(G7,G28,G12,G15,G16,G17,G21,G18,G27)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:119" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="87">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2490,11 +2557,19 @@
       <c r="H19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="96"/>
+      <c r="J19" s="33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR19" s="55">
+        <f>SUM(G13,G19,G20,G22,G24,G26)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="87">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2520,11 +2595,17 @@
       <c r="H20" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="I20" s="33" t="s">
+      <c r="I20" s="95"/>
+      <c r="J20" s="33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:118" s="36" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AQ20" s="3"/>
+      <c r="AR20" s="56" t="e">
+        <f>SUM(AR16:AR19)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:119" s="36" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="87">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2550,10 +2631,10 @@
       <c r="H21" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I21" s="68"/>
+      <c r="J21" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="52"/>
       <c r="K21" s="52"/>
       <c r="L21" s="52"/>
       <c r="M21" s="52"/>
@@ -2586,8 +2667,8 @@
       <c r="AN21" s="52"/>
       <c r="AO21" s="52"/>
       <c r="AP21" s="52"/>
-      <c r="AQ21" s="52"/>
-      <c r="AR21" s="52"/>
+      <c r="AQ21" s="4"/>
+      <c r="AR21" s="57"/>
       <c r="AS21" s="52"/>
       <c r="AT21" s="52"/>
       <c r="AU21" s="52"/>
@@ -2662,8 +2743,9 @@
       <c r="DL21" s="52"/>
       <c r="DM21" s="52"/>
       <c r="DN21" s="52"/>
-    </row>
-    <row r="22" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO21" s="52"/>
+    </row>
+    <row r="22" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="87">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2689,10 +2771,10 @@
       <c r="H22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="96"/>
+      <c r="J22" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="52"/>
       <c r="K22" s="52"/>
       <c r="L22" s="52"/>
       <c r="M22" s="52"/>
@@ -2801,8 +2883,9 @@
       <c r="DL22" s="52"/>
       <c r="DM22" s="52"/>
       <c r="DN22" s="52"/>
-    </row>
-    <row r="23" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO22" s="52"/>
+    </row>
+    <row r="23" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="87">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2828,10 +2911,10 @@
       <c r="H23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="96"/>
+      <c r="J23" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="52"/>
       <c r="K23" s="52"/>
       <c r="L23" s="52"/>
       <c r="M23" s="52"/>
@@ -2940,8 +3023,9 @@
       <c r="DL23" s="52"/>
       <c r="DM23" s="52"/>
       <c r="DN23" s="52"/>
-    </row>
-    <row r="24" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO23" s="52"/>
+    </row>
+    <row r="24" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="87">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2949,7 +3033,9 @@
       <c r="B24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" s="14" t="s">
         <v>3</v>
       </c>
@@ -2965,10 +3051,10 @@
       <c r="H24" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="65" t="s">
+      <c r="I24" s="77"/>
+      <c r="J24" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="52"/>
       <c r="K24" s="52"/>
       <c r="L24" s="52"/>
       <c r="M24" s="52"/>
@@ -3077,8 +3163,9 @@
       <c r="DL24" s="52"/>
       <c r="DM24" s="52"/>
       <c r="DN24" s="52"/>
-    </row>
-    <row r="25" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO24" s="52"/>
+    </row>
+    <row r="25" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="87">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3104,10 +3191,10 @@
       <c r="H25" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="I25" s="65" t="s">
+      <c r="I25" s="77"/>
+      <c r="J25" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="52"/>
       <c r="K25" s="52"/>
       <c r="L25" s="52"/>
       <c r="M25" s="52"/>
@@ -3216,8 +3303,9 @@
       <c r="DL25" s="52"/>
       <c r="DM25" s="52"/>
       <c r="DN25" s="52"/>
-    </row>
-    <row r="26" spans="1:118" s="36" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO25" s="52"/>
+    </row>
+    <row r="26" spans="1:119" s="36" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="87">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3243,10 +3331,10 @@
       <c r="H26" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="I26" s="65" t="s">
+      <c r="I26" s="77"/>
+      <c r="J26" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="52"/>
       <c r="K26" s="52"/>
       <c r="L26" s="52"/>
       <c r="M26" s="52"/>
@@ -3355,8 +3443,9 @@
       <c r="DL26" s="52"/>
       <c r="DM26" s="52"/>
       <c r="DN26" s="52"/>
-    </row>
-    <row r="27" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO26" s="52"/>
+    </row>
+    <row r="27" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="87">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3364,7 +3453,9 @@
       <c r="B27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="D27" s="14" t="s">
         <v>3</v>
       </c>
@@ -3380,10 +3471,10 @@
       <c r="H27" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="66" t="s">
+      <c r="I27" s="98"/>
+      <c r="J27" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="52"/>
       <c r="K27" s="52"/>
       <c r="L27" s="52"/>
       <c r="M27" s="52"/>
@@ -3492,8 +3583,9 @@
       <c r="DL27" s="52"/>
       <c r="DM27" s="52"/>
       <c r="DN27" s="52"/>
-    </row>
-    <row r="28" spans="1:118" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="DO27" s="52"/>
+    </row>
+    <row r="28" spans="1:119" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="87">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3517,12 +3609,13 @@
       <c r="H28" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I28" s="37" t="s">
+      <c r="I28" s="96"/>
+      <c r="J28" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="87">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3534,9 +3627,10 @@
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
       <c r="H29" s="93"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I29" s="99"/>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="87">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3548,9 +3642,10 @@
       <c r="F30" s="21"/>
       <c r="G30" s="11"/>
       <c r="H30" s="7"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I30" s="96"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="87">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3562,9 +3657,10 @@
       <c r="F31" s="21"/>
       <c r="G31" s="14"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="33"/>
-    </row>
-    <row r="32" spans="1:118" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I31" s="96"/>
+      <c r="J31" s="33"/>
+    </row>
+    <row r="32" spans="1:119" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="89">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3576,9 +3672,10 @@
       <c r="F32" s="71"/>
       <c r="G32" s="63"/>
       <c r="H32" s="72"/>
-      <c r="I32" s="73"/>
-    </row>
-    <row r="33" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="100"/>
+      <c r="J32" s="73"/>
+    </row>
+    <row r="33" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="89">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3590,9 +3687,10 @@
       <c r="F33" s="71"/>
       <c r="G33" s="63"/>
       <c r="H33" s="77"/>
-      <c r="I33" s="78"/>
-    </row>
-    <row r="34" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I33" s="77"/>
+      <c r="J33" s="78"/>
+    </row>
+    <row r="34" spans="1:10" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="89">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3604,9 +3702,10 @@
       <c r="F34" s="71"/>
       <c r="G34" s="63"/>
       <c r="H34" s="77"/>
-      <c r="I34" s="79"/>
-    </row>
-    <row r="35" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I34" s="77"/>
+      <c r="J34" s="79"/>
+    </row>
+    <row r="35" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="88">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3618,9 +3717,10 @@
       <c r="F35" s="80"/>
       <c r="G35" s="80"/>
       <c r="H35" s="80"/>
-      <c r="I35" s="81"/>
-    </row>
-    <row r="36" spans="1:9" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="80"/>
+      <c r="J35" s="81"/>
+    </row>
+    <row r="36" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="88">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3632,9 +3732,10 @@
       <c r="F36" s="80"/>
       <c r="G36" s="80"/>
       <c r="H36" s="80"/>
-      <c r="I36" s="50"/>
-    </row>
-    <row r="37" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="80"/>
+      <c r="J36" s="50"/>
+    </row>
+    <row r="37" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="88">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3646,9 +3747,10 @@
       <c r="F37" s="80"/>
       <c r="G37" s="80"/>
       <c r="H37" s="80"/>
-      <c r="I37" s="50"/>
-    </row>
-    <row r="38" spans="1:9" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I37" s="80"/>
+      <c r="J37" s="50"/>
+    </row>
+    <row r="38" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="91">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3660,9 +3762,10 @@
       <c r="F38" s="80"/>
       <c r="G38" s="80"/>
       <c r="H38" s="80"/>
-      <c r="I38" s="34"/>
-    </row>
-    <row r="39" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I38" s="80"/>
+      <c r="J38" s="34"/>
+    </row>
+    <row r="39" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="80"/>
       <c r="B39" s="80"/>
       <c r="C39" s="80"/>
@@ -3672,7 +3775,7 @@
       <c r="G39" s="80"/>
       <c r="H39" s="86"/>
     </row>
-    <row r="40" spans="1:9" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="80"/>
       <c r="B40" s="80"/>
       <c r="C40" s="80"/>
@@ -3682,7 +3785,7 @@
       <c r="G40" s="80"/>
       <c r="H40" s="86"/>
     </row>
-    <row r="41" spans="1:9" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="80"/>
       <c r="B41" s="80"/>
       <c r="C41" s="80"/>
@@ -3699,6 +3802,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -3708,23 +3812,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678EE90E01C1554D81095FA0DFA567B7" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="83375873e153ee88e233d36814b94c56">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e7a52f9-5c66-44a9-86f3-38766607b952" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16774528b49d9f4162b8bb368f2e4e5f" ns3:_="">
     <xsd:import namespace="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
@@ -3912,31 +3999,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA5CB000-8B96-4BBE-9725-8A7879A4E0C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92BE042B-9643-4CF1-BCF5-0B9BB1BB178C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E2715CD-D1C5-41E7-B27F-52AD5F236090}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3952,4 +4032,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92BE042B-9643-4CF1-BCF5-0B9BB1BB178C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA5CB000-8B96-4BBE-9725-8A7879A4E0C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>